<commit_message>
Generacion de la base de inversiones mediante la API creación de la clase inversiones
</commit_message>
<xml_diff>
--- a/Indices_Sectores.xlsx
+++ b/Indices_Sectores.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://planeacionnacional-my.sharepoint.com/personal/ucd_dnp_gov_co/Documents/Repositorio UCD/Proyectos UCD/2024/P27-2024_Mapa_brechas/Codigo/Source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{A0BA2B74-CE98-4CA7-BF09-C80143DEADBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{774A82E3-6EA4-43DE-A0DC-3E65E6C1F4B4}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="8_{A0BA2B74-CE98-4CA7-BF09-C80143DEADBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1BB4869A-5745-4FF0-B6AA-6918FF6351D4}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{54C9D73C-B1D9-4BB3-ABED-861DA94693BB}"/>
   </bookViews>
@@ -470,12 +470,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -491,6 +490,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -812,18 +815,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F7E0498-DC7F-4F5C-96DC-0B4364E4F182}">
   <dimension ref="A1:B115"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="G100" sqref="G100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" customWidth="1"/>
     <col min="2" max="2" width="50.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" t="s">
         <v>131</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -831,7 +834,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
         <v>129</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -839,7 +842,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" t="s">
         <v>128</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -847,7 +850,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" t="s">
         <v>127</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -855,7 +858,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" t="s">
         <v>126</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -863,7 +866,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" t="s">
         <v>125</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -871,7 +874,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="A7" t="s">
         <v>124</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -879,7 +882,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="A8" t="s">
         <v>123</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -887,7 +890,7 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="A9" t="s">
         <v>122</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -895,7 +898,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="A10" t="s">
         <v>121</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -903,7 +906,7 @@
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+      <c r="A11" t="s">
         <v>120</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -911,7 +914,7 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+      <c r="A12" t="s">
         <v>119</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -919,7 +922,7 @@
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+      <c r="A13" t="s">
         <v>118</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -927,7 +930,7 @@
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
+      <c r="A14" t="s">
         <v>117</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -935,7 +938,7 @@
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+      <c r="A15" t="s">
         <v>116</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -943,7 +946,7 @@
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+      <c r="A16" t="s">
         <v>115</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -951,7 +954,7 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+      <c r="A17" t="s">
         <v>114</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -959,7 +962,7 @@
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+      <c r="A18" t="s">
         <v>113</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -967,7 +970,7 @@
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+      <c r="A19" t="s">
         <v>112</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -975,7 +978,7 @@
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+      <c r="A20" t="s">
         <v>111</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -983,7 +986,7 @@
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
+      <c r="A21" t="s">
         <v>110</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -991,7 +994,7 @@
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
+      <c r="A22" t="s">
         <v>109</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -999,7 +1002,7 @@
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
+      <c r="A23" t="s">
         <v>108</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -1007,7 +1010,7 @@
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
+      <c r="A24" t="s">
         <v>107</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -1015,7 +1018,7 @@
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
+      <c r="A25" t="s">
         <v>106</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -1023,7 +1026,7 @@
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
+      <c r="A26" t="s">
         <v>105</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -1031,7 +1034,7 @@
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
+      <c r="A27" t="s">
         <v>104</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -1039,7 +1042,7 @@
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
+      <c r="A28" t="s">
         <v>103</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -1047,7 +1050,7 @@
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
+      <c r="A29" t="s">
         <v>102</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -1055,7 +1058,7 @@
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
+      <c r="A30" t="s">
         <v>101</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -1063,7 +1066,7 @@
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
+      <c r="A31" t="s">
         <v>100</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -1071,7 +1074,7 @@
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
+      <c r="A32" t="s">
         <v>99</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -1079,7 +1082,7 @@
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
+      <c r="A33" t="s">
         <v>98</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -1087,7 +1090,7 @@
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
+      <c r="A34" t="s">
         <v>96</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -1095,7 +1098,7 @@
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
+      <c r="A35" t="s">
         <v>95</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -1103,7 +1106,7 @@
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="2" t="s">
+      <c r="A36" t="s">
         <v>94</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -1111,7 +1114,7 @@
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="2" t="s">
+      <c r="A37" t="s">
         <v>93</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -1119,7 +1122,7 @@
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" s="2" t="s">
+      <c r="A38" t="s">
         <v>92</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -1127,7 +1130,7 @@
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" s="2" t="s">
+      <c r="A39" t="s">
         <v>91</v>
       </c>
       <c r="B39" s="1" t="s">
@@ -1135,7 +1138,7 @@
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" s="2" t="s">
+      <c r="A40" t="s">
         <v>90</v>
       </c>
       <c r="B40" s="1" t="s">
@@ -1143,7 +1146,7 @@
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="2" t="s">
+      <c r="A41" t="s">
         <v>89</v>
       </c>
       <c r="B41" s="1" t="s">
@@ -1151,7 +1154,7 @@
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" s="2" t="s">
+      <c r="A42" t="s">
         <v>88</v>
       </c>
       <c r="B42" s="1" t="s">
@@ -1159,7 +1162,7 @@
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="2" t="s">
+      <c r="A43" t="s">
         <v>87</v>
       </c>
       <c r="B43" s="1" t="s">
@@ -1167,7 +1170,7 @@
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" s="2" t="s">
+      <c r="A44" t="s">
         <v>85</v>
       </c>
       <c r="B44" s="1" t="s">
@@ -1175,7 +1178,7 @@
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" s="2" t="s">
+      <c r="A45" t="s">
         <v>86</v>
       </c>
       <c r="B45" s="1" t="s">
@@ -1183,7 +1186,7 @@
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" s="2" t="s">
+      <c r="A46" t="s">
         <v>85</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -1191,7 +1194,7 @@
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" s="2" t="s">
+      <c r="A47" t="s">
         <v>84</v>
       </c>
       <c r="B47" s="1" t="s">
@@ -1199,7 +1202,7 @@
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" s="2" t="s">
+      <c r="A48" t="s">
         <v>83</v>
       </c>
       <c r="B48" s="1" t="s">
@@ -1207,7 +1210,7 @@
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" s="2" t="s">
+      <c r="A49" t="s">
         <v>82</v>
       </c>
       <c r="B49" s="1" t="s">
@@ -1215,7 +1218,7 @@
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" s="2" t="s">
+      <c r="A50" t="s">
         <v>81</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -1223,7 +1226,7 @@
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" s="2" t="s">
+      <c r="A51" t="s">
         <v>80</v>
       </c>
       <c r="B51" s="1" t="s">
@@ -1231,7 +1234,7 @@
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" s="2" t="s">
+      <c r="A52" t="s">
         <v>79</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -1239,7 +1242,7 @@
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53" s="2" t="s">
+      <c r="A53" t="s">
         <v>78</v>
       </c>
       <c r="B53" s="1" t="s">
@@ -1247,7 +1250,7 @@
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" s="2" t="s">
+      <c r="A54" t="s">
         <v>77</v>
       </c>
       <c r="B54" s="1" t="s">
@@ -1255,7 +1258,7 @@
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55" s="2" t="s">
+      <c r="A55" t="s">
         <v>75</v>
       </c>
       <c r="B55" s="1" t="s">
@@ -1263,7 +1266,7 @@
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A56" s="2" t="s">
+      <c r="A56" t="s">
         <v>74</v>
       </c>
       <c r="B56" s="1" t="s">
@@ -1271,7 +1274,7 @@
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A57" s="2" t="s">
+      <c r="A57" t="s">
         <v>73</v>
       </c>
       <c r="B57" s="1" t="s">
@@ -1279,7 +1282,7 @@
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58" s="2" t="s">
+      <c r="A58" t="s">
         <v>72</v>
       </c>
       <c r="B58" s="1" t="s">
@@ -1287,7 +1290,7 @@
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A59" s="2" t="s">
+      <c r="A59" t="s">
         <v>71</v>
       </c>
       <c r="B59" s="1" t="s">
@@ -1295,7 +1298,7 @@
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A60" s="2" t="s">
+      <c r="A60" t="s">
         <v>70</v>
       </c>
       <c r="B60" s="1" t="s">
@@ -1303,7 +1306,7 @@
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61" s="2" t="s">
+      <c r="A61" t="s">
         <v>69</v>
       </c>
       <c r="B61" s="1" t="s">
@@ -1311,7 +1314,7 @@
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A62" s="2" t="s">
+      <c r="A62" t="s">
         <v>68</v>
       </c>
       <c r="B62" s="1" t="s">
@@ -1319,7 +1322,7 @@
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A63" s="2" t="s">
+      <c r="A63" t="s">
         <v>67</v>
       </c>
       <c r="B63" s="1" t="s">
@@ -1327,7 +1330,7 @@
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A64" s="2" t="s">
+      <c r="A64" t="s">
         <v>66</v>
       </c>
       <c r="B64" s="1" t="s">
@@ -1335,7 +1338,7 @@
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A65" s="2" t="s">
+      <c r="A65" t="s">
         <v>65</v>
       </c>
       <c r="B65" s="1" t="s">
@@ -1343,7 +1346,7 @@
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A66" s="2" t="s">
+      <c r="A66" t="s">
         <v>64</v>
       </c>
       <c r="B66" s="1" t="s">
@@ -1351,7 +1354,7 @@
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A67" s="2" t="s">
+      <c r="A67" t="s">
         <v>63</v>
       </c>
       <c r="B67" s="1" t="s">
@@ -1359,7 +1362,7 @@
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A68" s="2" t="s">
+      <c r="A68" t="s">
         <v>62</v>
       </c>
       <c r="B68" s="1" t="s">
@@ -1367,7 +1370,7 @@
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A69" s="2" t="s">
+      <c r="A69" t="s">
         <v>61</v>
       </c>
       <c r="B69" s="1" t="s">
@@ -1375,7 +1378,7 @@
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A70" s="2" t="s">
+      <c r="A70" t="s">
         <v>59</v>
       </c>
       <c r="B70" s="1" t="s">
@@ -1383,7 +1386,7 @@
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A71" s="2" t="s">
+      <c r="A71" t="s">
         <v>58</v>
       </c>
       <c r="B71" s="1" t="s">
@@ -1391,7 +1394,7 @@
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A72" s="2" t="s">
+      <c r="A72" t="s">
         <v>57</v>
       </c>
       <c r="B72" s="1" t="s">
@@ -1399,7 +1402,7 @@
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A73" s="2" t="s">
+      <c r="A73" t="s">
         <v>56</v>
       </c>
       <c r="B73" s="1" t="s">
@@ -1407,7 +1410,7 @@
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A74" s="2" t="s">
+      <c r="A74" t="s">
         <v>55</v>
       </c>
       <c r="B74" s="1" t="s">
@@ -1415,7 +1418,7 @@
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A75" s="2" t="s">
+      <c r="A75" t="s">
         <v>54</v>
       </c>
       <c r="B75" s="1" t="s">
@@ -1423,7 +1426,7 @@
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A76" s="2" t="s">
+      <c r="A76" t="s">
         <v>53</v>
       </c>
       <c r="B76" s="1" t="s">
@@ -1431,7 +1434,7 @@
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A77" s="2" t="s">
+      <c r="A77" t="s">
         <v>51</v>
       </c>
       <c r="B77" s="1" t="s">
@@ -1439,7 +1442,7 @@
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A78" s="2" t="s">
+      <c r="A78" t="s">
         <v>50</v>
       </c>
       <c r="B78" s="1" t="s">
@@ -1447,7 +1450,7 @@
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A79" s="2" t="s">
+      <c r="A79" t="s">
         <v>49</v>
       </c>
       <c r="B79" s="1" t="s">
@@ -1455,7 +1458,7 @@
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A80" s="2" t="s">
+      <c r="A80" t="s">
         <v>48</v>
       </c>
       <c r="B80" s="1" t="s">
@@ -1463,7 +1466,7 @@
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A81" s="2" t="s">
+      <c r="A81" t="s">
         <v>47</v>
       </c>
       <c r="B81" s="1" t="s">
@@ -1471,7 +1474,7 @@
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A82" s="2" t="s">
+      <c r="A82" t="s">
         <v>46</v>
       </c>
       <c r="B82" s="1" t="s">
@@ -1479,7 +1482,7 @@
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A83" s="2" t="s">
+      <c r="A83" t="s">
         <v>44</v>
       </c>
       <c r="B83" s="1" t="s">
@@ -1487,7 +1490,7 @@
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A84" s="2" t="s">
+      <c r="A84" t="s">
         <v>42</v>
       </c>
       <c r="B84" s="1" t="s">
@@ -1495,7 +1498,7 @@
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A85" s="2" t="s">
+      <c r="A85" t="s">
         <v>41</v>
       </c>
       <c r="B85" s="1" t="s">
@@ -1503,7 +1506,7 @@
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A86" s="2" t="s">
+      <c r="A86" t="s">
         <v>40</v>
       </c>
       <c r="B86" s="1" t="s">
@@ -1511,7 +1514,7 @@
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A87" s="2" t="s">
+      <c r="A87" t="s">
         <v>39</v>
       </c>
       <c r="B87" s="1" t="s">
@@ -1519,7 +1522,7 @@
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A88" s="2" t="s">
+      <c r="A88" t="s">
         <v>38</v>
       </c>
       <c r="B88" s="1" t="s">
@@ -1527,7 +1530,7 @@
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A89" s="2" t="s">
+      <c r="A89" t="s">
         <v>37</v>
       </c>
       <c r="B89" s="1" t="s">
@@ -1535,7 +1538,7 @@
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A90" s="2" t="s">
+      <c r="A90" t="s">
         <v>36</v>
       </c>
       <c r="B90" s="1" t="s">
@@ -1543,7 +1546,7 @@
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A91" s="2" t="s">
+      <c r="A91" t="s">
         <v>35</v>
       </c>
       <c r="B91" s="1" t="s">
@@ -1551,7 +1554,7 @@
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A92" s="2" t="s">
+      <c r="A92" t="s">
         <v>33</v>
       </c>
       <c r="B92" s="1" t="s">
@@ -1559,7 +1562,7 @@
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A93" s="2" t="s">
+      <c r="A93" t="s">
         <v>32</v>
       </c>
       <c r="B93" s="1" t="s">
@@ -1567,7 +1570,7 @@
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A94" s="2" t="s">
+      <c r="A94" t="s">
         <v>30</v>
       </c>
       <c r="B94" s="1" t="s">
@@ -1575,7 +1578,7 @@
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A95" s="2" t="s">
+      <c r="A95" t="s">
         <v>28</v>
       </c>
       <c r="B95" s="1" t="s">
@@ -1583,7 +1586,7 @@
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A96" s="2" t="s">
+      <c r="A96" t="s">
         <v>27</v>
       </c>
       <c r="B96" s="1" t="s">
@@ -1591,7 +1594,7 @@
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A97" s="2" t="s">
+      <c r="A97" t="s">
         <v>26</v>
       </c>
       <c r="B97" s="1" t="s">
@@ -1599,7 +1602,7 @@
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A98" s="2" t="s">
+      <c r="A98" t="s">
         <v>24</v>
       </c>
       <c r="B98" s="1" t="s">
@@ -1607,7 +1610,7 @@
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A99" s="2" t="s">
+      <c r="A99" t="s">
         <v>23</v>
       </c>
       <c r="B99" s="1" t="s">
@@ -1615,7 +1618,7 @@
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A100" s="2" t="s">
+      <c r="A100" t="s">
         <v>22</v>
       </c>
       <c r="B100" s="1" t="s">
@@ -1623,7 +1626,7 @@
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A101" s="2" t="s">
+      <c r="A101" t="s">
         <v>21</v>
       </c>
       <c r="B101" s="1" t="s">
@@ -1631,7 +1634,7 @@
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A102" s="2" t="s">
+      <c r="A102" t="s">
         <v>20</v>
       </c>
       <c r="B102" s="1" t="s">
@@ -1639,7 +1642,7 @@
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A103" s="2" t="s">
+      <c r="A103" t="s">
         <v>19</v>
       </c>
       <c r="B103" s="1" t="s">
@@ -1647,7 +1650,7 @@
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A104" s="2" t="s">
+      <c r="A104" t="s">
         <v>18</v>
       </c>
       <c r="B104" s="1" t="s">
@@ -1655,7 +1658,7 @@
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A105" s="2" t="s">
+      <c r="A105" t="s">
         <v>17</v>
       </c>
       <c r="B105" s="1" t="s">
@@ -1663,7 +1666,7 @@
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A106" s="2" t="s">
+      <c r="A106" t="s">
         <v>15</v>
       </c>
       <c r="B106" s="1" t="s">
@@ -1671,7 +1674,7 @@
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A107" s="2" t="s">
+      <c r="A107" t="s">
         <v>13</v>
       </c>
       <c r="B107" s="1" t="s">
@@ -1679,7 +1682,7 @@
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A108" s="2" t="s">
+      <c r="A108" t="s">
         <v>11</v>
       </c>
       <c r="B108" s="1" t="s">
@@ -1687,7 +1690,7 @@
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A109" s="2" t="s">
+      <c r="A109" t="s">
         <v>10</v>
       </c>
       <c r="B109" s="1" t="s">
@@ -1695,7 +1698,7 @@
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A110" s="2" t="s">
+      <c r="A110" t="s">
         <v>8</v>
       </c>
       <c r="B110" s="1" t="s">
@@ -1703,7 +1706,7 @@
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A111" s="2" t="s">
+      <c r="A111" t="s">
         <v>6</v>
       </c>
       <c r="B111" s="1" t="s">
@@ -1711,7 +1714,7 @@
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A112" s="2" t="s">
+      <c r="A112" t="s">
         <v>5</v>
       </c>
       <c r="B112" s="1" t="s">
@@ -1719,7 +1722,7 @@
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A113" s="2" t="s">
+      <c r="A113" t="s">
         <v>4</v>
       </c>
       <c r="B113" s="1" t="s">
@@ -1727,7 +1730,7 @@
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A114" s="2" t="s">
+      <c r="A114" t="s">
         <v>2</v>
       </c>
       <c r="B114" s="1" t="s">
@@ -1735,7 +1738,7 @@
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A115" s="2" t="s">
+      <c r="A115" t="s">
         <v>1</v>
       </c>
       <c r="B115" s="1" t="s">

</xml_diff>